<commit_message>
Update example files to match oca-data-vault:0.2.3
</commit_message>
<xml_diff>
--- a/examples/swiss_passport/digital_passport.xlsx
+++ b/examples/swiss_passport/digital_passport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -801,7 +801,7 @@
     <t xml:space="preserve">utf-8</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:EWSSp1MZQfVWl-u4l4eDprRp-bLE-xLe0gSTNVwkuqNA</t>
+    <t xml:space="preserve">SAI:EGyWgdQR9dW_I5oHlHBMoO9AA_eMeb2p3XzcCRCBbKCM</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
@@ -849,7 +849,7 @@
     <t xml:space="preserve">nationality</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:EcOqelFTDay0reu_CesOIUfWVF7htg4IvSOrrXuIMaXU</t>
+    <t xml:space="preserve">SAI:EmXip-eMwEeLWH9_AfH642_Zb-oGZXk7jI49qafz_XrU</t>
   </si>
   <si>
     <t xml:space="preserve">dateOfBirth</t>
@@ -933,7 +933,7 @@
     <t xml:space="preserve">Mandatory header|Issuing State or organization (in full)</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:ECfBoOwdcHhQfNtWA5qTKOo9egoxHKXxby6R8Jujpk-o</t>
+    <t xml:space="preserve">SAI:Els6NxGvFfyL5aiBWR3j7YiaS7F4j4O-F0EIlZu-dO0g</t>
   </si>
   <si>
     <t xml:space="preserve">The name of the State or organization responsible for issuing the MRP shall be displayed in full.</t>
@@ -957,7 +957,7 @@
     <t xml:space="preserve">Mandatory header|Issuing State or organization (in code)</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:EnmO60xL2IsIv-_AC2PgLdJtzqsfuNqa8BihsiNWgz5o</t>
+    <t xml:space="preserve">SAI:EdxqlME_1Zt0Y_YJ3c0uMIzd41mSDATbH-rp7ElqhNes</t>
   </si>
   <si>
     <t xml:space="preserve">As abbreviated in the three-letter code specified in Doc 9303-3.</t>
@@ -990,7 +990,7 @@
     <t xml:space="preserve">Mandatory and optional personal data elements|Nationality</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:EAr0uvi1743P2VXXqd08a-yX8K_aejHCkdjaW8lWZ_xw</t>
+    <t xml:space="preserve">SAI:EXdSkFdYnAzZ2U2Qyo-q76CJMYelgV9NXN8GhmtY2ErY</t>
   </si>
   <si>
     <t xml:space="preserve">For details see Doc 9303-3.</t>
@@ -1059,7 +1059,7 @@
     <t xml:space="preserve">Mandatory identification feature|Identification feature</t>
   </si>
   <si>
-    <t xml:space="preserve">This field shall contain a portrait of the holder. The portrait shall not be larger than 45.0 mm x 35.0 mm_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000B_(1.77 in x 1.38 in) nor smaller than 32.0 mm x 26.0 mm (1.26 in x 1.02 in). The position of the field concerned shall be aligned to the left of Zones II, III and IV. See Doc 9303-3 for additional specifications for the portrait.</t>
+    <t xml:space="preserve">This field shall contain a portrait of the holder. The portrait shall not be larger than 45.0 mm x 35.0 mm_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000B_(1.77 in x 1.38 in) nor smaller than 32.0 mm x 26.0 mm (1.26 in x 1.02 in). The position of the field concerned shall be aligned to the left of Zones II, III and IV. See Doc 9303-3 for additional specifications for the portrait.</t>
   </si>
   <si>
     <t xml:space="preserve">Optional data elements|Optional data elements</t>
@@ -1101,7 +1101,7 @@
     <t xml:space="preserve">En-tête obligatoire|État ou organisme émetteur (au complet)</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:EL_PI1HJ7qyGdT3yrH7kXqwWAv0-lxGLXEtzN8C6zQt4</t>
+    <t xml:space="preserve">SAI:Emj736NIuEKdR-3sfXB4wfPokFzgE7uiRm6EXKaJRyE4</t>
   </si>
   <si>
     <t xml:space="preserve">Le nom de l'État ou de l'organisme responsable de la délivrance du MRP doit être indiqué en toutes lettres.</t>
@@ -1155,7 +1155,7 @@
     <t xml:space="preserve">Éléments de données personnelles obligatoires et facultatifs|Nationalité</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:E3iUl-Nc2Tb1d-LBuCsd1JJJH1ppjFtIxYyX7_VB_d3c</t>
+    <t xml:space="preserve">SAI:Ez_5-oggNDr7gUFaz3GSof1y579gK0MKXIVesRjGzyqY</t>
   </si>
   <si>
     <t xml:space="preserve">Pour plus de détails, voir Doc 9303-3.</t>
@@ -2873,9 +2873,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>121320</xdr:colOff>
+      <xdr:colOff>120960</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2889,7 +2889,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4060440" y="281880"/>
-          <a:ext cx="2902320" cy="822600"/>
+          <a:ext cx="2901960" cy="822240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4488,8 +4488,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4585,7 +4585,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" s="66" customFormat="true" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="66" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="59" t="s">
         <v>88</v>
       </c>
@@ -4776,7 +4776,7 @@
       <c r="I11" s="72"/>
       <c r="J11" s="74"/>
     </row>
-    <row r="12" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="77" t="s">
         <v>88</v>
       </c>
@@ -5100,7 +5100,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5164,7 +5164,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="94" t="s">
         <v>4</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="98" t="s">
         <v>4</v>
       </c>
@@ -5570,8 +5570,8 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5629,7 +5629,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="94" t="s">
         <v>188</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="98" t="s">
         <v>188</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="98" t="s">
         <v>188</v>
       </c>

</xml_diff>

<commit_message>
Remove mapping overlays from examples/swiss_passport/digital_passport.xlsx
</commit_message>
<xml_diff>
--- a/examples/swiss_passport/digital_passport.xlsx
+++ b/examples/swiss_passport/digital_passport.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="234">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -873,9 +873,6 @@
     <t xml:space="preserve">F|M|X</t>
   </si>
   <si>
-    <t xml:space="preserve">F:K|X:unknown</t>
-  </si>
-  <si>
     <t xml:space="preserve">placeOfBirth</t>
   </si>
   <si>
@@ -885,9 +882,6 @@
     <t xml:space="preserve">SI|cm</t>
   </si>
   <si>
-    <t xml:space="preserve">height</t>
-  </si>
-  <si>
     <t xml:space="preserve">dateOfIssue</t>
   </si>
   <si>
@@ -1062,7 +1056,7 @@
     <t xml:space="preserve">Mandatory identification feature|Identification feature</t>
   </si>
   <si>
-    <t xml:space="preserve">This field shall contain a portrait of the holder. The portrait shall not be larger than 45.0 mm x 35.0 mm_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000B_(1.77 in x 1.38 in) nor smaller than 32.0 mm x 26.0 mm (1.26 in x 1.02 in). The position of the field concerned shall be aligned to the left of Zones II, III and IV. See Doc 9303-3 for additional specifications for the portrait.</t>
+    <t xml:space="preserve">This field shall contain a portrait of the holder. The portrait shall not be larger than 45.0 mm x 35.0 mm_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000B_(1.77 in x 1.38 in) nor smaller than 32.0 mm x 26.0 mm (1.26 in x 1.02 in). The position of the field concerned shall be aligned to the left of Zones II, III and IV. See Doc 9303-3 for additional specifications for the portrait.</t>
   </si>
   <si>
     <t xml:space="preserve">Optional data elements|Optional data elements</t>
@@ -2876,9 +2870,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>120600</xdr:colOff>
+      <xdr:colOff>120240</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2892,7 +2886,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4060800" y="282240"/>
-          <a:ext cx="2901240" cy="821520"/>
+          <a:ext cx="2900880" cy="821160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4591,8 +4585,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4968,16 +4962,13 @@
       <c r="H15" s="72"/>
       <c r="I15" s="72"/>
       <c r="J15" s="74"/>
-      <c r="N15" s="0" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="77" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" s="69" t="s">
         <v>56</v>
@@ -4999,7 +4990,7 @@
         <v>88</v>
       </c>
       <c r="B17" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="69" t="s">
         <v>56</v>
@@ -5016,10 +5007,7 @@
       <c r="I17" s="72"/>
       <c r="J17" s="74"/>
       <c r="L17" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5015,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" s="69" t="s">
         <v>109</v>
@@ -5049,7 +5037,7 @@
         <v>88</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" s="69" t="s">
         <v>56</v>
@@ -5069,7 +5057,7 @@
         <v>88</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C20" s="69" t="s">
         <v>109</v>
@@ -5091,7 +5079,7 @@
         <v>88</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C21" s="69" t="s">
         <v>56</v>
@@ -5113,19 +5101,19 @@
         <v>88</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D22" s="70" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F22" s="72" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G22" s="78"/>
       <c r="H22" s="72"/>
@@ -5137,19 +5125,19 @@
         <v>88</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D23" s="70" t="s">
         <v>101</v>
       </c>
       <c r="E23" s="71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F23" s="72" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G23" s="78"/>
       <c r="H23" s="72"/>
@@ -5161,7 +5149,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C24" s="80" t="s">
         <v>56</v>
@@ -5226,10 +5214,10 @@
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="89" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F1" s="90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5238,18 +5226,18 @@
       <c r="C2" s="92"/>
       <c r="D2" s="52"/>
       <c r="E2" s="55" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="93" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" s="89" t="s">
         <v>23</v>
@@ -5269,19 +5257,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="59" t="s">
         <v>89</v>
       </c>
       <c r="D4" s="96" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="96" t="s">
         <v>135</v>
-      </c>
-      <c r="E4" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="96" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,19 +5277,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" s="68" t="s">
         <v>93</v>
       </c>
       <c r="D5" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="100" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="68" t="s">
         <v>138</v>
-      </c>
-      <c r="E5" s="100" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5309,17 +5297,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>95</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" s="100"/>
       <c r="F6" s="68" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5327,19 +5315,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C7" s="68" t="s">
         <v>98</v>
       </c>
       <c r="D7" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="100" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="68" t="s">
         <v>143</v>
-      </c>
-      <c r="E7" s="100" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="68" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,17 +5335,17 @@
         <v>4</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>100</v>
       </c>
       <c r="D8" s="68" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5365,17 +5353,17 @@
         <v>4</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" s="68" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="68" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,17 +5371,17 @@
         <v>4</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C10" s="68" t="s">
         <v>104</v>
       </c>
       <c r="D10" s="68" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E10" s="100"/>
       <c r="F10" s="68" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5401,17 +5389,17 @@
         <v>4</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11" s="68" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E11" s="100"/>
       <c r="F11" s="68" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5419,19 +5407,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C12" s="68" t="s">
         <v>106</v>
       </c>
       <c r="D12" s="68" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="100" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="68" t="s">
         <v>154</v>
-      </c>
-      <c r="E12" s="100" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="68" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5439,17 +5427,17 @@
         <v>4</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" s="68" t="s">
         <v>108</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E13" s="100"/>
       <c r="F13" s="68" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5457,17 +5445,17 @@
         <v>4</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C14" s="68" t="s">
         <v>111</v>
       </c>
       <c r="D14" s="68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E14" s="100"/>
       <c r="F14" s="68" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5475,19 +5463,19 @@
         <v>4</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C15" s="68" t="s">
         <v>113</v>
       </c>
       <c r="D15" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="100" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="68" t="s">
         <v>161</v>
-      </c>
-      <c r="E15" s="100" t="s">
-        <v>162</v>
-      </c>
-      <c r="F15" s="68" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5495,17 +5483,17 @@
         <v>4</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C16" s="68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="68" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E16" s="100"/>
       <c r="F16" s="68" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5513,17 +5501,17 @@
         <v>4</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C17" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="68" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E17" s="100"/>
       <c r="F17" s="68" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5531,17 +5519,17 @@
         <v>4</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C18" s="68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D18" s="68" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E18" s="100"/>
       <c r="F18" s="68" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5549,17 +5537,17 @@
         <v>4</v>
       </c>
       <c r="B19" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" s="68" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E19" s="100"/>
       <c r="F19" s="68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5567,17 +5555,17 @@
         <v>4</v>
       </c>
       <c r="B20" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" s="68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D20" s="68" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E20" s="100"/>
       <c r="F20" s="68" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5585,17 +5573,17 @@
         <v>4</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" s="68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D21" s="68" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E21" s="100"/>
       <c r="F21" s="68" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,17 +5591,17 @@
         <v>4</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D22" s="68" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E22" s="100"/>
       <c r="F22" s="68" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5621,17 +5609,17 @@
         <v>4</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C23" s="68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D23" s="68" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E23" s="100"/>
       <c r="F23" s="68" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5639,17 +5627,17 @@
         <v>4</v>
       </c>
       <c r="B24" s="102" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C24" s="79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D24" s="79" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E24" s="103"/>
       <c r="F24" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5690,10 +5678,10 @@
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
       <c r="E1" s="93" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F1" s="104" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5702,418 +5690,418 @@
       <c r="C2" s="105"/>
       <c r="D2" s="91"/>
       <c r="E2" s="106" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F2" s="107" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="93" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="D3" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="E3" s="93" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="F3" s="104" t="s">
         <v>186</v>
-      </c>
-      <c r="E3" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="F3" s="104" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="94" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" s="59" t="s">
         <v>89</v>
       </c>
       <c r="D4" s="96" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="97" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="96" t="s">
         <v>191</v>
-      </c>
-      <c r="E4" s="97" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="96" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C5" s="68" t="s">
         <v>93</v>
       </c>
       <c r="D5" s="68" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="100" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="68" t="s">
         <v>194</v>
-      </c>
-      <c r="E5" s="100" t="s">
-        <v>195</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>95</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E6" s="100"/>
       <c r="F6" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="68" t="s">
         <v>98</v>
       </c>
       <c r="D7" s="68" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" s="100" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>100</v>
       </c>
       <c r="D8" s="68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E8" s="100"/>
       <c r="F8" s="68" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C9" s="68" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="68" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="68" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C10" s="68" t="s">
         <v>104</v>
       </c>
       <c r="D10" s="68" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E10" s="100"/>
       <c r="F10" s="68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B11" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C11" s="68" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="68" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E11" s="100"/>
       <c r="F11" s="68" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C12" s="68" t="s">
         <v>106</v>
       </c>
       <c r="D12" s="68" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="100" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="68" t="s">
         <v>209</v>
-      </c>
-      <c r="E12" s="100" t="s">
-        <v>210</v>
-      </c>
-      <c r="F12" s="68" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C13" s="68" t="s">
         <v>108</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E13" s="100"/>
       <c r="F13" s="68" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C14" s="68" t="s">
         <v>111</v>
       </c>
       <c r="D14" s="68" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E14" s="100"/>
       <c r="F14" s="68" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B15" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C15" s="68" t="s">
         <v>113</v>
       </c>
       <c r="D15" s="68" t="s">
+        <v>214</v>
+      </c>
+      <c r="E15" s="100" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="68" t="s">
         <v>216</v>
-      </c>
-      <c r="E15" s="100" t="s">
-        <v>217</v>
-      </c>
-      <c r="F15" s="68" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C16" s="68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="68" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E16" s="100"/>
       <c r="F16" s="68" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B17" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C17" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="68" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E17" s="100"/>
       <c r="F17" s="68" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B18" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C18" s="68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D18" s="68" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E18" s="100"/>
       <c r="F18" s="68" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B19" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D19" s="68" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E19" s="100"/>
       <c r="F19" s="68" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B20" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C20" s="68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D20" s="68" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E20" s="100"/>
       <c r="F20" s="68" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C21" s="68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D21" s="68" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E21" s="100"/>
       <c r="F21" s="68" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D22" s="68" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E22" s="100"/>
       <c r="F22" s="68" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="98" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B23" s="99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C23" s="68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D23" s="68" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E23" s="100"/>
       <c r="F23" s="68" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="101" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B24" s="102" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C24" s="79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D24" s="79" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E24" s="103"/>
       <c r="F24" s="79" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>